<commit_message>
add gitignore, add route, add itemIcon
</commit_message>
<xml_diff>
--- a/DataSource/excel/Item.xlsx
+++ b/DataSource/excel/Item.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="960" windowWidth="24640" windowHeight="13920" tabRatio="500"/>
+    <workbookView xWindow="960" yWindow="960" windowWidth="24640" windowHeight="13860" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="team.csv" sheetId="1" r:id="rId1"/>
+    <sheet name="Item.csv" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -18,200 +18,44 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Yujie Liu</author>
-  </authors>
-  <commentList>
-    <comment ref="A1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Yujie Liu:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-1. </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="2"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">物品表， 有两个description，和id绑定，就不一一写了
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Yujie Liu:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-1:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="2"/>
-            <charset val="134"/>
-          </rPr>
-          <t>武器
-2：防具
-3：装备品
-4：道具
-5：航海用具
-6：其他
-7：地图</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Yujie Liu:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="2"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">职务
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
+    <t>itemId</t>
+  </si>
+  <si>
+    <t>iconId</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>job</t>
+  </si>
+  <si>
     <t>id</t>
   </si>
   <si>
     <t>string</t>
   </si>
   <si>
-    <t>itemId</t>
-  </si>
-  <si>
-    <t>iconId</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
     <t>int</t>
-  </si>
-  <si>
-    <t>value</t>
-  </si>
-  <si>
-    <t>job</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="宋体"/>
-      <family val="2"/>
-      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -231,21 +75,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="5">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -574,53 +410,85 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>133</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>30</v>
+      </c>
+      <c r="E3">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>134</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>40</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
minor change of item panel, make dialog to use easier
</commit_message>
<xml_diff>
--- a/DataSource/excel/Item.xlsx
+++ b/DataSource/excel/Item.xlsx
@@ -18,8 +18,57 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Yujie Liu</author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yujie Liu:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+1</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="2"/>
+            <charset val="134"/>
+          </rPr>
+          <t>武器
+2防具
+3装备
+4航海用品
+5其他
+6地图和证</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>itemId</t>
   </si>
@@ -43,19 +92,100 @@
   </si>
   <si>
     <t>int</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>南瓜种子</t>
+  </si>
+  <si>
+    <t>番茄苗</t>
+  </si>
+  <si>
+    <t>香蕉树</t>
+  </si>
+  <si>
+    <t>蜜蜂窝</t>
+  </si>
+  <si>
+    <t>鲨鱼幼鱼</t>
+  </si>
+  <si>
+    <t>胡椒粒</t>
+  </si>
+  <si>
+    <t>丁香粒</t>
+  </si>
+  <si>
+    <t>金黄色猫</t>
+  </si>
+  <si>
+    <t>莱姆汁</t>
+  </si>
+  <si>
+    <t>赫密士的祈祷</t>
+  </si>
+  <si>
+    <t>华佗的中药</t>
+  </si>
+  <si>
+    <t>漆黑的双刃长剑</t>
+  </si>
+  <si>
+    <t>拉奥孔剑</t>
+  </si>
+  <si>
+    <t>苍蓝橡木盾</t>
+  </si>
+  <si>
+    <t>魔法的皮手套</t>
+  </si>
+  <si>
+    <t>穿山甲的铁皮</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -78,8 +208,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,41 +541,47 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -452,43 +589,333 @@
       <c r="E2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>133</v>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>134</v>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
         <v>2</v>
       </c>
-      <c r="D4">
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10">
+        <v>20</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11">
+        <v>21</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12">
+        <v>22</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13">
+        <v>23</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14">
+        <v>24</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>24</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15">
+        <v>25</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>34</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16">
+        <v>49</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>24</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17">
+        <v>50</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>18</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18">
+        <v>74</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18">
         <v>40</v>
       </c>
-      <c r="E4">
+      <c r="F18">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Add equip job and value for the item and use default dialog to buy/sell items
</commit_message>
<xml_diff>
--- a/DataSource/excel/Item.xlsx
+++ b/DataSource/excel/Item.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3560" yWindow="620" windowWidth="24640" windowHeight="13860" tabRatio="500"/>
+    <workbookView xWindow="6980" yWindow="100" windowWidth="18960" windowHeight="13820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Item.csv" sheetId="1" r:id="rId1"/>
@@ -109,12 +109,46 @@
         </r>
       </text>
     </comment>
+    <comment ref="I1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yujie Liu:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="2"/>
+            <charset val="134"/>
+          </rPr>
+          <t>每一个道具都是唯一的，所以cityId和guildId只可能有一个</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="222">
   <si>
     <t>itemId</t>
   </si>
@@ -774,6 +808,12 @@
   </si>
   <si>
     <t>琼恰克的王冠</t>
+  </si>
+  <si>
+    <t>ownerCityId</t>
+  </si>
+  <si>
+    <t>ownerGuildId</t>
   </si>
 </sst>
 </file>
@@ -849,8 +889,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -860,11 +912,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1194,18 +1258,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H210"/>
+  <dimension ref="A1:J210"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="G117" sqref="G117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1230,8 +1295,14 @@
       <c r="H1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" t="s">
+        <v>220</v>
+      </c>
+      <c r="J1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1256,8 +1327,14 @@
       <c r="H2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1283,8 +1360,14 @@
       <c r="H3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1310,8 +1393,14 @@
       <c r="H4">
         <v>1100</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1337,8 +1426,14 @@
       <c r="H5">
         <v>1200</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1364,8 +1459,14 @@
       <c r="H6">
         <v>1300</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1391,8 +1492,14 @@
       <c r="H7">
         <v>1400</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1418,8 +1525,14 @@
       <c r="H8">
         <v>1500</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1445,8 +1558,14 @@
       <c r="H9">
         <v>1600</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1472,8 +1591,14 @@
       <c r="H10">
         <v>1600</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1499,8 +1624,14 @@
       <c r="H11">
         <v>1600</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1526,8 +1657,14 @@
       <c r="H12">
         <v>1600</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1553,8 +1690,14 @@
       <c r="H13">
         <v>1600</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1580,8 +1723,14 @@
       <c r="H14">
         <v>1600</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1607,8 +1756,14 @@
       <c r="H15">
         <v>1600</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1634,8 +1789,14 @@
       <c r="H16">
         <v>1600</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1661,8 +1822,14 @@
       <c r="H17">
         <v>1600</v>
       </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1688,8 +1855,14 @@
       <c r="H18">
         <v>1600</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1715,8 +1888,14 @@
       <c r="H19">
         <v>1600</v>
       </c>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1742,8 +1921,14 @@
       <c r="H20">
         <v>1600</v>
       </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1769,8 +1954,14 @@
       <c r="H21">
         <v>1600</v>
       </c>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1796,8 +1987,14 @@
       <c r="H22">
         <v>1600</v>
       </c>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1823,8 +2020,14 @@
       <c r="H23">
         <v>1700</v>
       </c>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1850,8 +2053,14 @@
       <c r="H24">
         <v>1800</v>
       </c>
-    </row>
-    <row r="25" spans="1:8">
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1877,8 +2086,14 @@
       <c r="H25">
         <v>1900</v>
       </c>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1904,8 +2119,14 @@
       <c r="H26">
         <v>2000</v>
       </c>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1931,8 +2152,14 @@
       <c r="H27">
         <v>2100</v>
       </c>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1958,8 +2185,14 @@
       <c r="H28">
         <v>2200</v>
       </c>
-    </row>
-    <row r="29" spans="1:8">
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1985,8 +2218,14 @@
       <c r="H29">
         <v>2300</v>
       </c>
-    </row>
-    <row r="30" spans="1:8">
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30">
         <v>28</v>
       </c>
@@ -2012,8 +2251,14 @@
       <c r="H30">
         <v>2400</v>
       </c>
-    </row>
-    <row r="31" spans="1:8">
+      <c r="I30">
+        <v>1</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31">
         <v>29</v>
       </c>
@@ -2039,8 +2284,14 @@
       <c r="H31">
         <v>2500</v>
       </c>
-    </row>
-    <row r="32" spans="1:8">
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32">
         <v>30</v>
       </c>
@@ -2066,8 +2317,14 @@
       <c r="H32">
         <v>2600</v>
       </c>
-    </row>
-    <row r="33" spans="1:8">
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33">
         <v>31</v>
       </c>
@@ -2093,8 +2350,14 @@
       <c r="H33">
         <v>2700</v>
       </c>
-    </row>
-    <row r="34" spans="1:8">
+      <c r="I33">
+        <v>1</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34">
         <v>32</v>
       </c>
@@ -2120,8 +2383,14 @@
       <c r="H34">
         <v>2800</v>
       </c>
-    </row>
-    <row r="35" spans="1:8">
+      <c r="I34">
+        <v>1</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35">
         <v>33</v>
       </c>
@@ -2147,8 +2416,14 @@
       <c r="H35">
         <v>2900</v>
       </c>
-    </row>
-    <row r="36" spans="1:8">
+      <c r="I35">
+        <v>1</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36">
         <v>34</v>
       </c>
@@ -2174,8 +2449,14 @@
       <c r="H36">
         <v>3000</v>
       </c>
-    </row>
-    <row r="37" spans="1:8">
+      <c r="I36">
+        <v>1</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37">
         <v>35</v>
       </c>
@@ -2201,8 +2482,14 @@
       <c r="H37">
         <v>3100</v>
       </c>
-    </row>
-    <row r="38" spans="1:8">
+      <c r="I37">
+        <v>1</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38">
         <v>36</v>
       </c>
@@ -2228,8 +2515,14 @@
       <c r="H38">
         <v>3200</v>
       </c>
-    </row>
-    <row r="39" spans="1:8">
+      <c r="I38">
+        <v>1</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39">
         <v>37</v>
       </c>
@@ -2255,8 +2548,14 @@
       <c r="H39">
         <v>3300</v>
       </c>
-    </row>
-    <row r="40" spans="1:8">
+      <c r="I39">
+        <v>1</v>
+      </c>
+      <c r="J39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40">
         <v>38</v>
       </c>
@@ -2282,8 +2581,14 @@
       <c r="H40">
         <v>3400</v>
       </c>
-    </row>
-    <row r="41" spans="1:8">
+      <c r="I40">
+        <v>1</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41">
         <v>39</v>
       </c>
@@ -2309,8 +2614,14 @@
       <c r="H41">
         <v>3500</v>
       </c>
-    </row>
-    <row r="42" spans="1:8">
+      <c r="I41">
+        <v>1</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42">
         <v>40</v>
       </c>
@@ -2336,8 +2647,14 @@
       <c r="H42">
         <v>3600</v>
       </c>
-    </row>
-    <row r="43" spans="1:8">
+      <c r="I42">
+        <v>1</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43">
         <v>41</v>
       </c>
@@ -2363,8 +2680,14 @@
       <c r="H43">
         <v>3700</v>
       </c>
-    </row>
-    <row r="44" spans="1:8">
+      <c r="I43">
+        <v>1</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44">
         <v>42</v>
       </c>
@@ -2390,8 +2713,14 @@
       <c r="H44">
         <v>3800</v>
       </c>
-    </row>
-    <row r="45" spans="1:8">
+      <c r="I44">
+        <v>1</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45">
         <v>43</v>
       </c>
@@ -2417,8 +2746,14 @@
       <c r="H45">
         <v>3900</v>
       </c>
-    </row>
-    <row r="46" spans="1:8">
+      <c r="I45">
+        <v>1</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
       <c r="A46">
         <v>44</v>
       </c>
@@ -2444,8 +2779,14 @@
       <c r="H46">
         <v>4000</v>
       </c>
-    </row>
-    <row r="47" spans="1:8">
+      <c r="I46">
+        <v>1</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
       <c r="A47">
         <v>45</v>
       </c>
@@ -2471,8 +2812,14 @@
       <c r="H47">
         <v>4100</v>
       </c>
-    </row>
-    <row r="48" spans="1:8">
+      <c r="I47">
+        <v>1</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
       <c r="A48">
         <v>46</v>
       </c>
@@ -2498,8 +2845,14 @@
       <c r="H48">
         <v>4200</v>
       </c>
-    </row>
-    <row r="49" spans="1:8">
+      <c r="I48">
+        <v>1</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
       <c r="A49">
         <v>47</v>
       </c>
@@ -2525,8 +2878,14 @@
       <c r="H49">
         <v>4300</v>
       </c>
-    </row>
-    <row r="50" spans="1:8">
+      <c r="I49">
+        <v>1</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
       <c r="A50">
         <v>48</v>
       </c>
@@ -2552,8 +2911,14 @@
       <c r="H50">
         <v>4400</v>
       </c>
-    </row>
-    <row r="51" spans="1:8">
+      <c r="I50">
+        <v>1</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
       <c r="A51">
         <v>49</v>
       </c>
@@ -2579,8 +2944,14 @@
       <c r="H51">
         <v>4500</v>
       </c>
-    </row>
-    <row r="52" spans="1:8">
+      <c r="I51">
+        <v>1</v>
+      </c>
+      <c r="J51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
       <c r="A52">
         <v>50</v>
       </c>
@@ -2606,8 +2977,14 @@
       <c r="H52">
         <v>4600</v>
       </c>
-    </row>
-    <row r="53" spans="1:8">
+      <c r="I52">
+        <v>1</v>
+      </c>
+      <c r="J52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
       <c r="A53">
         <v>51</v>
       </c>
@@ -2633,8 +3010,14 @@
       <c r="H53">
         <v>4700</v>
       </c>
-    </row>
-    <row r="54" spans="1:8">
+      <c r="I53">
+        <v>1</v>
+      </c>
+      <c r="J53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
       <c r="A54">
         <v>52</v>
       </c>
@@ -2660,8 +3043,14 @@
       <c r="H54">
         <v>4800</v>
       </c>
-    </row>
-    <row r="55" spans="1:8">
+      <c r="I54">
+        <v>1</v>
+      </c>
+      <c r="J54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
       <c r="A55">
         <v>53</v>
       </c>
@@ -2687,8 +3076,14 @@
       <c r="H55">
         <v>4900</v>
       </c>
-    </row>
-    <row r="56" spans="1:8">
+      <c r="I55">
+        <v>1</v>
+      </c>
+      <c r="J55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
       <c r="A56">
         <v>54</v>
       </c>
@@ -2714,8 +3109,14 @@
       <c r="H56">
         <v>5000</v>
       </c>
-    </row>
-    <row r="57" spans="1:8">
+      <c r="I56">
+        <v>1</v>
+      </c>
+      <c r="J56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
       <c r="A57">
         <v>55</v>
       </c>
@@ -2741,8 +3142,14 @@
       <c r="H57">
         <v>5100</v>
       </c>
-    </row>
-    <row r="58" spans="1:8">
+      <c r="I57">
+        <v>1</v>
+      </c>
+      <c r="J57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
       <c r="A58">
         <v>56</v>
       </c>
@@ -2768,8 +3175,14 @@
       <c r="H58">
         <v>5200</v>
       </c>
-    </row>
-    <row r="59" spans="1:8">
+      <c r="I58">
+        <v>1</v>
+      </c>
+      <c r="J58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
       <c r="A59">
         <v>57</v>
       </c>
@@ -2795,8 +3208,14 @@
       <c r="H59">
         <v>5300</v>
       </c>
-    </row>
-    <row r="60" spans="1:8">
+      <c r="I59">
+        <v>1</v>
+      </c>
+      <c r="J59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
       <c r="A60">
         <v>58</v>
       </c>
@@ -2822,8 +3241,14 @@
       <c r="H60">
         <v>5400</v>
       </c>
-    </row>
-    <row r="61" spans="1:8">
+      <c r="I60">
+        <v>1</v>
+      </c>
+      <c r="J60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
       <c r="A61">
         <v>59</v>
       </c>
@@ -2849,8 +3274,14 @@
       <c r="H61">
         <v>5500</v>
       </c>
-    </row>
-    <row r="62" spans="1:8">
+      <c r="I61">
+        <v>1</v>
+      </c>
+      <c r="J61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
       <c r="A62">
         <v>60</v>
       </c>
@@ -2876,8 +3307,14 @@
       <c r="H62">
         <v>5600</v>
       </c>
-    </row>
-    <row r="63" spans="1:8">
+      <c r="I62">
+        <v>1</v>
+      </c>
+      <c r="J62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
       <c r="A63">
         <v>61</v>
       </c>
@@ -2903,8 +3340,14 @@
       <c r="H63">
         <v>5700</v>
       </c>
-    </row>
-    <row r="64" spans="1:8">
+      <c r="I63">
+        <v>1</v>
+      </c>
+      <c r="J63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
       <c r="A64">
         <v>62</v>
       </c>
@@ -2930,8 +3373,14 @@
       <c r="H64">
         <v>5800</v>
       </c>
-    </row>
-    <row r="65" spans="1:8">
+      <c r="I64">
+        <v>1</v>
+      </c>
+      <c r="J64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
       <c r="A65">
         <v>63</v>
       </c>
@@ -2957,8 +3406,14 @@
       <c r="H65">
         <v>5900</v>
       </c>
-    </row>
-    <row r="66" spans="1:8">
+      <c r="I65">
+        <v>1</v>
+      </c>
+      <c r="J65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
       <c r="A66">
         <v>64</v>
       </c>
@@ -2984,8 +3439,14 @@
       <c r="H66">
         <v>6000</v>
       </c>
-    </row>
-    <row r="67" spans="1:8">
+      <c r="I66">
+        <v>1</v>
+      </c>
+      <c r="J66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
       <c r="A67">
         <v>65</v>
       </c>
@@ -3011,8 +3472,14 @@
       <c r="H67">
         <v>6100</v>
       </c>
-    </row>
-    <row r="68" spans="1:8">
+      <c r="I67">
+        <v>1</v>
+      </c>
+      <c r="J67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
       <c r="A68">
         <v>66</v>
       </c>
@@ -3023,7 +3490,7 @@
         <v>65</v>
       </c>
       <c r="D68">
-        <f t="shared" ref="D68:D131" si="1">E68</f>
+        <f t="shared" ref="D68:D129" si="1">E68</f>
         <v>2</v>
       </c>
       <c r="E68">
@@ -3038,8 +3505,14 @@
       <c r="H68">
         <v>6200</v>
       </c>
-    </row>
-    <row r="69" spans="1:8">
+      <c r="I68">
+        <v>1</v>
+      </c>
+      <c r="J68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
       <c r="A69">
         <v>67</v>
       </c>
@@ -3065,8 +3538,14 @@
       <c r="H69">
         <v>6300</v>
       </c>
-    </row>
-    <row r="70" spans="1:8">
+      <c r="I69">
+        <v>1</v>
+      </c>
+      <c r="J69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
       <c r="A70">
         <v>68</v>
       </c>
@@ -3092,8 +3571,14 @@
       <c r="H70">
         <v>6400</v>
       </c>
-    </row>
-    <row r="71" spans="1:8">
+      <c r="I70">
+        <v>1</v>
+      </c>
+      <c r="J70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10">
       <c r="A71">
         <v>69</v>
       </c>
@@ -3119,8 +3604,14 @@
       <c r="H71">
         <v>6500</v>
       </c>
-    </row>
-    <row r="72" spans="1:8">
+      <c r="I71">
+        <v>1</v>
+      </c>
+      <c r="J71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10">
       <c r="A72">
         <v>70</v>
       </c>
@@ -3146,8 +3637,14 @@
       <c r="H72">
         <v>6600</v>
       </c>
-    </row>
-    <row r="73" spans="1:8">
+      <c r="I72">
+        <v>1</v>
+      </c>
+      <c r="J72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10">
       <c r="A73">
         <v>71</v>
       </c>
@@ -3173,8 +3670,14 @@
       <c r="H73">
         <v>6700</v>
       </c>
-    </row>
-    <row r="74" spans="1:8">
+      <c r="I73">
+        <v>1</v>
+      </c>
+      <c r="J73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10">
       <c r="A74">
         <v>72</v>
       </c>
@@ -3200,8 +3703,14 @@
       <c r="H74">
         <v>6800</v>
       </c>
-    </row>
-    <row r="75" spans="1:8">
+      <c r="I74">
+        <v>1</v>
+      </c>
+      <c r="J74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10">
       <c r="A75">
         <v>73</v>
       </c>
@@ -3227,8 +3736,14 @@
       <c r="H75">
         <v>6900</v>
       </c>
-    </row>
-    <row r="76" spans="1:8">
+      <c r="I75">
+        <v>1</v>
+      </c>
+      <c r="J75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10">
       <c r="A76">
         <v>74</v>
       </c>
@@ -3254,8 +3769,14 @@
       <c r="H76">
         <v>7000</v>
       </c>
-    </row>
-    <row r="77" spans="1:8">
+      <c r="I76">
+        <v>1</v>
+      </c>
+      <c r="J76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10">
       <c r="A77">
         <v>75</v>
       </c>
@@ -3276,13 +3797,19 @@
         <v>40</v>
       </c>
       <c r="G77">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H77">
         <v>7100</v>
       </c>
-    </row>
-    <row r="78" spans="1:8">
+      <c r="I77">
+        <v>1</v>
+      </c>
+      <c r="J77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10">
       <c r="A78">
         <v>76</v>
       </c>
@@ -3303,13 +3830,19 @@
         <v>54</v>
       </c>
       <c r="G78">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H78">
         <v>7200</v>
       </c>
-    </row>
-    <row r="79" spans="1:8">
+      <c r="I78">
+        <v>1</v>
+      </c>
+      <c r="J78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10">
       <c r="A79">
         <v>77</v>
       </c>
@@ -3330,13 +3863,19 @@
         <v>32</v>
       </c>
       <c r="G79">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H79">
         <v>7300</v>
       </c>
-    </row>
-    <row r="80" spans="1:8">
+      <c r="I79">
+        <v>1</v>
+      </c>
+      <c r="J79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10">
       <c r="A80">
         <v>78</v>
       </c>
@@ -3357,13 +3896,19 @@
         <v>63</v>
       </c>
       <c r="G80">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H80">
         <v>7400</v>
       </c>
-    </row>
-    <row r="81" spans="1:8">
+      <c r="I80">
+        <v>1</v>
+      </c>
+      <c r="J80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10">
       <c r="A81">
         <v>79</v>
       </c>
@@ -3384,13 +3929,19 @@
         <v>34</v>
       </c>
       <c r="G81">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H81">
         <v>7500</v>
       </c>
-    </row>
-    <row r="82" spans="1:8">
+      <c r="I81">
+        <v>1</v>
+      </c>
+      <c r="J81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10">
       <c r="A82">
         <v>80</v>
       </c>
@@ -3411,13 +3962,19 @@
         <v>45</v>
       </c>
       <c r="G82">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H82">
         <v>7600</v>
       </c>
-    </row>
-    <row r="83" spans="1:8">
+      <c r="I82">
+        <v>1</v>
+      </c>
+      <c r="J82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10">
       <c r="A83">
         <v>81</v>
       </c>
@@ -3438,13 +3995,19 @@
         <v>12</v>
       </c>
       <c r="G83">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H83">
         <v>7700</v>
       </c>
-    </row>
-    <row r="84" spans="1:8">
+      <c r="I83">
+        <v>1</v>
+      </c>
+      <c r="J83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10">
       <c r="A84">
         <v>82</v>
       </c>
@@ -3465,13 +4028,19 @@
         <v>57</v>
       </c>
       <c r="G84">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H84">
         <v>7800</v>
       </c>
-    </row>
-    <row r="85" spans="1:8">
+      <c r="I84">
+        <v>1</v>
+      </c>
+      <c r="J84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10">
       <c r="A85">
         <v>83</v>
       </c>
@@ -3492,13 +4061,19 @@
         <v>18</v>
       </c>
       <c r="G85">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H85">
         <v>7900</v>
       </c>
-    </row>
-    <row r="86" spans="1:8">
+      <c r="I85">
+        <v>1</v>
+      </c>
+      <c r="J85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10">
       <c r="A86">
         <v>84</v>
       </c>
@@ -3519,13 +4094,19 @@
         <v>40</v>
       </c>
       <c r="G86">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H86">
         <v>8000</v>
       </c>
-    </row>
-    <row r="87" spans="1:8">
+      <c r="I86">
+        <v>1</v>
+      </c>
+      <c r="J86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10">
       <c r="A87">
         <v>85</v>
       </c>
@@ -3546,13 +4127,19 @@
         <v>50</v>
       </c>
       <c r="G87">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H87">
         <v>8100</v>
       </c>
-    </row>
-    <row r="88" spans="1:8">
+      <c r="I87">
+        <v>1</v>
+      </c>
+      <c r="J87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10">
       <c r="A88">
         <v>86</v>
       </c>
@@ -3573,13 +4160,19 @@
         <v>70</v>
       </c>
       <c r="G88">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H88">
         <v>8200</v>
       </c>
-    </row>
-    <row r="89" spans="1:8">
+      <c r="I88">
+        <v>1</v>
+      </c>
+      <c r="J88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10">
       <c r="A89">
         <v>87</v>
       </c>
@@ -3600,13 +4193,19 @@
         <v>35</v>
       </c>
       <c r="G89">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H89">
         <v>8300</v>
       </c>
-    </row>
-    <row r="90" spans="1:8">
+      <c r="I89">
+        <v>1</v>
+      </c>
+      <c r="J89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10">
       <c r="A90">
         <v>88</v>
       </c>
@@ -3627,13 +4226,19 @@
         <v>63</v>
       </c>
       <c r="G90">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H90">
         <v>8400</v>
       </c>
-    </row>
-    <row r="91" spans="1:8">
+      <c r="I90">
+        <v>1</v>
+      </c>
+      <c r="J90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10">
       <c r="A91">
         <v>89</v>
       </c>
@@ -3654,13 +4259,19 @@
         <v>34</v>
       </c>
       <c r="G91">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H91">
         <v>8500</v>
       </c>
-    </row>
-    <row r="92" spans="1:8">
+      <c r="I91">
+        <v>1</v>
+      </c>
+      <c r="J91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10">
       <c r="A92">
         <v>90</v>
       </c>
@@ -3681,13 +4292,19 @@
         <v>15</v>
       </c>
       <c r="G92">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H92">
         <v>8600</v>
       </c>
-    </row>
-    <row r="93" spans="1:8">
+      <c r="I92">
+        <v>1</v>
+      </c>
+      <c r="J92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10">
       <c r="A93">
         <v>91</v>
       </c>
@@ -3708,13 +4325,19 @@
         <v>40</v>
       </c>
       <c r="G93">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H93">
         <v>8700</v>
       </c>
-    </row>
-    <row r="94" spans="1:8">
+      <c r="I93">
+        <v>1</v>
+      </c>
+      <c r="J93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10">
       <c r="A94">
         <v>92</v>
       </c>
@@ -3735,13 +4358,19 @@
         <v>28</v>
       </c>
       <c r="G94">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H94">
         <v>8800</v>
       </c>
-    </row>
-    <row r="95" spans="1:8">
+      <c r="I94">
+        <v>1</v>
+      </c>
+      <c r="J94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10">
       <c r="A95">
         <v>93</v>
       </c>
@@ -3762,13 +4391,19 @@
         <v>32</v>
       </c>
       <c r="G95">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H95">
         <v>8900</v>
       </c>
-    </row>
-    <row r="96" spans="1:8">
+      <c r="I95">
+        <v>1</v>
+      </c>
+      <c r="J95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10">
       <c r="A96">
         <v>94</v>
       </c>
@@ -3789,13 +4424,19 @@
         <v>52</v>
       </c>
       <c r="G96">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H96">
         <v>9000</v>
       </c>
-    </row>
-    <row r="97" spans="1:8">
+      <c r="I96">
+        <v>1</v>
+      </c>
+      <c r="J96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10">
       <c r="A97">
         <v>95</v>
       </c>
@@ -3816,13 +4457,19 @@
         <v>47</v>
       </c>
       <c r="G97">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H97">
         <v>9100</v>
       </c>
-    </row>
-    <row r="98" spans="1:8">
+      <c r="I97">
+        <v>1</v>
+      </c>
+      <c r="J97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10">
       <c r="A98">
         <v>96</v>
       </c>
@@ -3843,13 +4490,19 @@
         <v>68</v>
       </c>
       <c r="G98">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H98">
         <v>9200</v>
       </c>
-    </row>
-    <row r="99" spans="1:8">
+      <c r="I98">
+        <v>1</v>
+      </c>
+      <c r="J98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10">
       <c r="A99">
         <v>97</v>
       </c>
@@ -3870,13 +4523,19 @@
         <v>32</v>
       </c>
       <c r="G99">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H99">
         <v>9300</v>
       </c>
-    </row>
-    <row r="100" spans="1:8">
+      <c r="I99">
+        <v>1</v>
+      </c>
+      <c r="J99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10">
       <c r="A100">
         <v>98</v>
       </c>
@@ -3897,13 +4556,19 @@
         <v>56</v>
       </c>
       <c r="G100">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H100">
         <v>9400</v>
       </c>
-    </row>
-    <row r="101" spans="1:8">
+      <c r="I100">
+        <v>1</v>
+      </c>
+      <c r="J100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10">
       <c r="A101">
         <v>99</v>
       </c>
@@ -3924,13 +4589,19 @@
         <v>21</v>
       </c>
       <c r="G101">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H101">
         <v>9500</v>
       </c>
-    </row>
-    <row r="102" spans="1:8">
+      <c r="I101">
+        <v>1</v>
+      </c>
+      <c r="J101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10">
       <c r="A102">
         <v>100</v>
       </c>
@@ -3951,13 +4622,19 @@
         <v>74</v>
       </c>
       <c r="G102">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="H102">
         <v>9600</v>
       </c>
-    </row>
-    <row r="103" spans="1:8">
+      <c r="I102">
+        <v>1</v>
+      </c>
+      <c r="J102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10">
       <c r="A103">
         <v>101</v>
       </c>
@@ -3978,13 +4655,19 @@
         <v>37</v>
       </c>
       <c r="G103">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="H103">
         <v>9700</v>
       </c>
-    </row>
-    <row r="104" spans="1:8">
+      <c r="I103">
+        <v>1</v>
+      </c>
+      <c r="J103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10">
       <c r="A104">
         <v>102</v>
       </c>
@@ -4005,13 +4688,19 @@
         <v>48</v>
       </c>
       <c r="G104">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="H104">
         <v>9800</v>
       </c>
-    </row>
-    <row r="105" spans="1:8">
+      <c r="I104">
+        <v>1</v>
+      </c>
+      <c r="J104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10">
       <c r="A105">
         <v>103</v>
       </c>
@@ -4032,13 +4721,19 @@
         <v>60</v>
       </c>
       <c r="G105">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H105">
         <v>9900</v>
       </c>
-    </row>
-    <row r="106" spans="1:8">
+      <c r="I105">
+        <v>1</v>
+      </c>
+      <c r="J105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10">
       <c r="A106">
         <v>104</v>
       </c>
@@ -4059,13 +4754,19 @@
         <v>20</v>
       </c>
       <c r="G106">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H106">
         <v>10000</v>
       </c>
-    </row>
-    <row r="107" spans="1:8">
+      <c r="I106">
+        <v>1</v>
+      </c>
+      <c r="J106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10">
       <c r="A107">
         <v>105</v>
       </c>
@@ -4086,13 +4787,19 @@
         <v>30</v>
       </c>
       <c r="G107">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="H107">
         <v>10100</v>
       </c>
-    </row>
-    <row r="108" spans="1:8">
+      <c r="I107">
+        <v>1</v>
+      </c>
+      <c r="J107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10">
       <c r="A108">
         <v>106</v>
       </c>
@@ -4113,13 +4820,19 @@
         <v>45</v>
       </c>
       <c r="G108">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="H108">
         <v>10200</v>
       </c>
-    </row>
-    <row r="109" spans="1:8">
+      <c r="I108">
+        <v>1</v>
+      </c>
+      <c r="J108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10">
       <c r="A109">
         <v>107</v>
       </c>
@@ -4140,13 +4853,19 @@
         <v>50</v>
       </c>
       <c r="G109">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="H109">
         <v>10300</v>
       </c>
-    </row>
-    <row r="110" spans="1:8">
+      <c r="I109">
+        <v>1</v>
+      </c>
+      <c r="J109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10">
       <c r="A110">
         <v>108</v>
       </c>
@@ -4167,13 +4886,19 @@
         <v>24</v>
       </c>
       <c r="G110">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="H110">
         <v>10400</v>
       </c>
-    </row>
-    <row r="111" spans="1:8">
+      <c r="I110">
+        <v>1</v>
+      </c>
+      <c r="J110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10">
       <c r="A111">
         <v>109</v>
       </c>
@@ -4194,13 +4919,19 @@
         <v>30</v>
       </c>
       <c r="G111">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="H111">
         <v>10500</v>
       </c>
-    </row>
-    <row r="112" spans="1:8">
+      <c r="I111">
+        <v>1</v>
+      </c>
+      <c r="J111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10">
       <c r="A112">
         <v>110</v>
       </c>
@@ -4221,13 +4952,19 @@
         <v>30</v>
       </c>
       <c r="G112">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H112">
         <v>10600</v>
       </c>
-    </row>
-    <row r="113" spans="1:8">
+      <c r="I112">
+        <v>1</v>
+      </c>
+      <c r="J112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10">
       <c r="A113">
         <v>111</v>
       </c>
@@ -4248,13 +4985,19 @@
         <v>45</v>
       </c>
       <c r="G113">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H113">
         <v>10700</v>
       </c>
-    </row>
-    <row r="114" spans="1:8">
+      <c r="I113">
+        <v>1</v>
+      </c>
+      <c r="J113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10">
       <c r="A114">
         <v>112</v>
       </c>
@@ -4275,13 +5018,19 @@
         <v>24</v>
       </c>
       <c r="G114">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H114">
         <v>10800</v>
       </c>
-    </row>
-    <row r="115" spans="1:8">
+      <c r="I114">
+        <v>1</v>
+      </c>
+      <c r="J114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10">
       <c r="A115">
         <v>113</v>
       </c>
@@ -4302,13 +5051,19 @@
         <v>39</v>
       </c>
       <c r="G115">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H115">
         <v>10900</v>
       </c>
-    </row>
-    <row r="116" spans="1:8">
+      <c r="I115">
+        <v>1</v>
+      </c>
+      <c r="J115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10">
       <c r="A116">
         <v>114</v>
       </c>
@@ -4329,13 +5084,19 @@
         <v>58</v>
       </c>
       <c r="G116">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H116">
         <v>11000</v>
       </c>
-    </row>
-    <row r="117" spans="1:8">
+      <c r="I116">
+        <v>1</v>
+      </c>
+      <c r="J116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10">
       <c r="A117">
         <v>115</v>
       </c>
@@ -4346,8 +5107,7 @@
         <v>114</v>
       </c>
       <c r="D117">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E117">
         <v>6</v>
@@ -4361,8 +5121,14 @@
       <c r="H117">
         <v>11100</v>
       </c>
-    </row>
-    <row r="118" spans="1:8">
+      <c r="I117">
+        <v>1</v>
+      </c>
+      <c r="J117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10">
       <c r="A118">
         <v>116</v>
       </c>
@@ -4373,8 +5139,7 @@
         <v>115</v>
       </c>
       <c r="D118">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E118">
         <v>6</v>
@@ -4388,8 +5153,14 @@
       <c r="H118">
         <v>11200</v>
       </c>
-    </row>
-    <row r="119" spans="1:8">
+      <c r="I118">
+        <v>1</v>
+      </c>
+      <c r="J118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10">
       <c r="A119">
         <v>117</v>
       </c>
@@ -4400,8 +5171,7 @@
         <v>116</v>
       </c>
       <c r="D119">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E119">
         <v>6</v>
@@ -4415,8 +5185,14 @@
       <c r="H119">
         <v>11300</v>
       </c>
-    </row>
-    <row r="120" spans="1:8">
+      <c r="I119">
+        <v>1</v>
+      </c>
+      <c r="J119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10">
       <c r="A120">
         <v>118</v>
       </c>
@@ -4427,8 +5203,7 @@
         <v>117</v>
       </c>
       <c r="D120">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E120">
         <v>6</v>
@@ -4442,8 +5217,14 @@
       <c r="H120">
         <v>11400</v>
       </c>
-    </row>
-    <row r="121" spans="1:8">
+      <c r="I120">
+        <v>1</v>
+      </c>
+      <c r="J120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10">
       <c r="A121">
         <v>119</v>
       </c>
@@ -4454,8 +5235,7 @@
         <v>118</v>
       </c>
       <c r="D121">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E121">
         <v>6</v>
@@ -4469,8 +5249,14 @@
       <c r="H121">
         <v>11500</v>
       </c>
-    </row>
-    <row r="122" spans="1:8">
+      <c r="I121">
+        <v>1</v>
+      </c>
+      <c r="J121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10">
       <c r="A122">
         <v>120</v>
       </c>
@@ -4481,8 +5267,7 @@
         <v>119</v>
       </c>
       <c r="D122">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E122">
         <v>6</v>
@@ -4496,8 +5281,14 @@
       <c r="H122">
         <v>11600</v>
       </c>
-    </row>
-    <row r="123" spans="1:8">
+      <c r="I122">
+        <v>1</v>
+      </c>
+      <c r="J122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10">
       <c r="A123">
         <v>121</v>
       </c>
@@ -4508,8 +5299,7 @@
         <v>120</v>
       </c>
       <c r="D123">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E123">
         <v>6</v>
@@ -4523,8 +5313,14 @@
       <c r="H123">
         <v>11700</v>
       </c>
-    </row>
-    <row r="124" spans="1:8">
+      <c r="I123">
+        <v>1</v>
+      </c>
+      <c r="J123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10">
       <c r="A124">
         <v>122</v>
       </c>
@@ -4535,8 +5331,7 @@
         <v>121</v>
       </c>
       <c r="D124">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E124">
         <v>6</v>
@@ -4550,8 +5345,14 @@
       <c r="H124">
         <v>11800</v>
       </c>
-    </row>
-    <row r="125" spans="1:8">
+      <c r="I124">
+        <v>1</v>
+      </c>
+      <c r="J124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10">
       <c r="A125">
         <v>123</v>
       </c>
@@ -4562,8 +5363,7 @@
         <v>122</v>
       </c>
       <c r="D125">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E125">
         <v>6</v>
@@ -4577,8 +5377,14 @@
       <c r="H125">
         <v>11900</v>
       </c>
-    </row>
-    <row r="126" spans="1:8">
+      <c r="I125">
+        <v>1</v>
+      </c>
+      <c r="J125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10">
       <c r="A126">
         <v>124</v>
       </c>
@@ -4589,8 +5395,7 @@
         <v>123</v>
       </c>
       <c r="D126">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E126">
         <v>6</v>
@@ -4604,8 +5409,14 @@
       <c r="H126">
         <v>12000</v>
       </c>
-    </row>
-    <row r="127" spans="1:8">
+      <c r="I126">
+        <v>1</v>
+      </c>
+      <c r="J126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10">
       <c r="A127">
         <v>125</v>
       </c>
@@ -4631,8 +5442,14 @@
       <c r="H127">
         <v>12100</v>
       </c>
-    </row>
-    <row r="128" spans="1:8">
+      <c r="I127">
+        <v>1</v>
+      </c>
+      <c r="J127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10">
       <c r="A128">
         <v>126</v>
       </c>
@@ -4658,8 +5475,14 @@
       <c r="H128">
         <v>12200</v>
       </c>
-    </row>
-    <row r="129" spans="1:8">
+      <c r="I128">
+        <v>1</v>
+      </c>
+      <c r="J128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10">
       <c r="A129">
         <v>127</v>
       </c>
@@ -4685,8 +5508,14 @@
       <c r="H129">
         <v>12300</v>
       </c>
-    </row>
-    <row r="130" spans="1:8">
+      <c r="I129">
+        <v>1</v>
+      </c>
+      <c r="J129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10">
       <c r="A130">
         <v>128</v>
       </c>
@@ -4711,8 +5540,14 @@
       <c r="H130">
         <v>12400</v>
       </c>
-    </row>
-    <row r="131" spans="1:8">
+      <c r="I130">
+        <v>1</v>
+      </c>
+      <c r="J130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10">
       <c r="A131">
         <v>129</v>
       </c>
@@ -4737,8 +5572,14 @@
       <c r="H131">
         <v>12500</v>
       </c>
-    </row>
-    <row r="132" spans="1:8">
+      <c r="I131">
+        <v>1</v>
+      </c>
+      <c r="J131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10">
       <c r="A132">
         <v>130</v>
       </c>
@@ -4763,8 +5604,14 @@
       <c r="H132">
         <v>12600</v>
       </c>
-    </row>
-    <row r="133" spans="1:8">
+      <c r="I132">
+        <v>1</v>
+      </c>
+      <c r="J132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10">
       <c r="A133">
         <v>131</v>
       </c>
@@ -4789,8 +5636,14 @@
       <c r="H133">
         <v>12700</v>
       </c>
-    </row>
-    <row r="134" spans="1:8">
+      <c r="I133">
+        <v>1</v>
+      </c>
+      <c r="J133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10">
       <c r="A134">
         <v>132</v>
       </c>
@@ -4815,8 +5668,14 @@
       <c r="H134">
         <v>12800</v>
       </c>
-    </row>
-    <row r="135" spans="1:8">
+      <c r="I134">
+        <v>1</v>
+      </c>
+      <c r="J134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10">
       <c r="A135">
         <v>133</v>
       </c>
@@ -4841,8 +5700,14 @@
       <c r="H135">
         <v>12900</v>
       </c>
-    </row>
-    <row r="136" spans="1:8">
+      <c r="I135">
+        <v>1</v>
+      </c>
+      <c r="J135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10">
       <c r="A136">
         <v>134</v>
       </c>
@@ -4867,8 +5732,14 @@
       <c r="H136">
         <v>13000</v>
       </c>
-    </row>
-    <row r="137" spans="1:8">
+      <c r="I136">
+        <v>1</v>
+      </c>
+      <c r="J136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10">
       <c r="A137">
         <v>135</v>
       </c>
@@ -4893,8 +5764,14 @@
       <c r="H137">
         <v>13100</v>
       </c>
-    </row>
-    <row r="138" spans="1:8">
+      <c r="I137">
+        <v>1</v>
+      </c>
+      <c r="J137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10">
       <c r="A138">
         <v>136</v>
       </c>
@@ -4919,8 +5796,14 @@
       <c r="H138">
         <v>13200</v>
       </c>
-    </row>
-    <row r="139" spans="1:8">
+      <c r="I138">
+        <v>1</v>
+      </c>
+      <c r="J138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10">
       <c r="A139">
         <v>137</v>
       </c>
@@ -4945,8 +5828,14 @@
       <c r="H139">
         <v>13300</v>
       </c>
-    </row>
-    <row r="140" spans="1:8">
+      <c r="I139">
+        <v>1</v>
+      </c>
+      <c r="J139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10">
       <c r="A140">
         <v>138</v>
       </c>
@@ -4971,8 +5860,14 @@
       <c r="H140">
         <v>13400</v>
       </c>
-    </row>
-    <row r="141" spans="1:8">
+      <c r="I140">
+        <v>1</v>
+      </c>
+      <c r="J140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10">
       <c r="A141">
         <v>139</v>
       </c>
@@ -4997,8 +5892,14 @@
       <c r="H141">
         <v>13500</v>
       </c>
-    </row>
-    <row r="142" spans="1:8">
+      <c r="I141">
+        <v>1</v>
+      </c>
+      <c r="J141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10">
       <c r="A142">
         <v>140</v>
       </c>
@@ -5023,8 +5924,14 @@
       <c r="H142">
         <v>13600</v>
       </c>
-    </row>
-    <row r="143" spans="1:8">
+      <c r="I142">
+        <v>1</v>
+      </c>
+      <c r="J142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10">
       <c r="A143">
         <v>141</v>
       </c>
@@ -5049,8 +5956,14 @@
       <c r="H143">
         <v>13700</v>
       </c>
-    </row>
-    <row r="144" spans="1:8">
+      <c r="I143">
+        <v>1</v>
+      </c>
+      <c r="J143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10">
       <c r="A144">
         <v>142</v>
       </c>
@@ -5075,8 +5988,14 @@
       <c r="H144">
         <v>13800</v>
       </c>
-    </row>
-    <row r="145" spans="1:8">
+      <c r="I144">
+        <v>1</v>
+      </c>
+      <c r="J144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10">
       <c r="A145">
         <v>143</v>
       </c>
@@ -5101,8 +6020,14 @@
       <c r="H145">
         <v>13900</v>
       </c>
-    </row>
-    <row r="146" spans="1:8">
+      <c r="I145">
+        <v>1</v>
+      </c>
+      <c r="J145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10">
       <c r="A146">
         <v>144</v>
       </c>
@@ -5127,8 +6052,14 @@
       <c r="H146">
         <v>14000</v>
       </c>
-    </row>
-    <row r="147" spans="1:8">
+      <c r="I146">
+        <v>1</v>
+      </c>
+      <c r="J146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10">
       <c r="A147">
         <v>145</v>
       </c>
@@ -5153,8 +6084,14 @@
       <c r="H147">
         <v>14100</v>
       </c>
-    </row>
-    <row r="148" spans="1:8">
+      <c r="I147">
+        <v>1</v>
+      </c>
+      <c r="J147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10">
       <c r="A148">
         <v>146</v>
       </c>
@@ -5179,8 +6116,14 @@
       <c r="H148">
         <v>14100</v>
       </c>
-    </row>
-    <row r="149" spans="1:8">
+      <c r="I148">
+        <v>1</v>
+      </c>
+      <c r="J148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10">
       <c r="A149">
         <v>147</v>
       </c>
@@ -5205,8 +6148,14 @@
       <c r="H149">
         <v>14100</v>
       </c>
-    </row>
-    <row r="150" spans="1:8">
+      <c r="I149">
+        <v>1</v>
+      </c>
+      <c r="J149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10">
       <c r="A150">
         <v>148</v>
       </c>
@@ -5231,8 +6180,14 @@
       <c r="H150">
         <v>14100</v>
       </c>
-    </row>
-    <row r="151" spans="1:8">
+      <c r="I150">
+        <v>1</v>
+      </c>
+      <c r="J150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10">
       <c r="A151">
         <v>149</v>
       </c>
@@ -5257,8 +6212,14 @@
       <c r="H151">
         <v>14100</v>
       </c>
-    </row>
-    <row r="152" spans="1:8">
+      <c r="I151">
+        <v>1</v>
+      </c>
+      <c r="J151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10">
       <c r="A152">
         <v>150</v>
       </c>
@@ -5283,8 +6244,14 @@
       <c r="H152">
         <v>14100</v>
       </c>
-    </row>
-    <row r="153" spans="1:8">
+      <c r="I152">
+        <v>1</v>
+      </c>
+      <c r="J152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10">
       <c r="A153">
         <v>151</v>
       </c>
@@ -5309,8 +6276,14 @@
       <c r="H153">
         <v>14100</v>
       </c>
-    </row>
-    <row r="154" spans="1:8">
+      <c r="I153">
+        <v>1</v>
+      </c>
+      <c r="J153">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10">
       <c r="A154">
         <v>152</v>
       </c>
@@ -5335,8 +6308,14 @@
       <c r="H154">
         <v>14100</v>
       </c>
-    </row>
-    <row r="155" spans="1:8">
+      <c r="I154">
+        <v>1</v>
+      </c>
+      <c r="J154">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10">
       <c r="A155">
         <v>153</v>
       </c>
@@ -5361,8 +6340,14 @@
       <c r="H155">
         <v>14100</v>
       </c>
-    </row>
-    <row r="156" spans="1:8">
+      <c r="I155">
+        <v>1</v>
+      </c>
+      <c r="J155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10">
       <c r="A156">
         <v>154</v>
       </c>
@@ -5387,8 +6372,14 @@
       <c r="H156">
         <v>14100</v>
       </c>
-    </row>
-    <row r="157" spans="1:8">
+      <c r="I156">
+        <v>1</v>
+      </c>
+      <c r="J156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10">
       <c r="A157">
         <v>155</v>
       </c>
@@ -5413,8 +6404,14 @@
       <c r="H157">
         <v>14100</v>
       </c>
-    </row>
-    <row r="158" spans="1:8">
+      <c r="I157">
+        <v>1</v>
+      </c>
+      <c r="J157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10">
       <c r="A158">
         <v>156</v>
       </c>
@@ -5439,8 +6436,14 @@
       <c r="H158">
         <v>14100</v>
       </c>
-    </row>
-    <row r="159" spans="1:8">
+      <c r="I158">
+        <v>1</v>
+      </c>
+      <c r="J158">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10">
       <c r="A159">
         <v>157</v>
       </c>
@@ -5465,8 +6468,14 @@
       <c r="H159">
         <v>14100</v>
       </c>
-    </row>
-    <row r="160" spans="1:8">
+      <c r="I159">
+        <v>1</v>
+      </c>
+      <c r="J159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10">
       <c r="A160">
         <v>158</v>
       </c>
@@ -5491,8 +6500,14 @@
       <c r="H160">
         <v>14100</v>
       </c>
-    </row>
-    <row r="161" spans="1:8">
+      <c r="I160">
+        <v>1</v>
+      </c>
+      <c r="J160">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10">
       <c r="A161">
         <v>159</v>
       </c>
@@ -5517,8 +6532,14 @@
       <c r="H161">
         <v>14100</v>
       </c>
-    </row>
-    <row r="162" spans="1:8">
+      <c r="I161">
+        <v>1</v>
+      </c>
+      <c r="J161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10">
       <c r="A162">
         <v>160</v>
       </c>
@@ -5543,8 +6564,14 @@
       <c r="H162">
         <v>14100</v>
       </c>
-    </row>
-    <row r="163" spans="1:8">
+      <c r="I162">
+        <v>1</v>
+      </c>
+      <c r="J162">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10">
       <c r="A163">
         <v>161</v>
       </c>
@@ -5569,8 +6596,14 @@
       <c r="H163">
         <v>14100</v>
       </c>
-    </row>
-    <row r="164" spans="1:8">
+      <c r="I163">
+        <v>1</v>
+      </c>
+      <c r="J163">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10">
       <c r="A164">
         <v>162</v>
       </c>
@@ -5595,8 +6628,14 @@
       <c r="H164">
         <v>14100</v>
       </c>
-    </row>
-    <row r="165" spans="1:8">
+      <c r="I164">
+        <v>1</v>
+      </c>
+      <c r="J164">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10">
       <c r="A165">
         <v>163</v>
       </c>
@@ -5621,8 +6660,14 @@
       <c r="H165">
         <v>14100</v>
       </c>
-    </row>
-    <row r="166" spans="1:8">
+      <c r="I165">
+        <v>1</v>
+      </c>
+      <c r="J165">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10">
       <c r="A166">
         <v>164</v>
       </c>
@@ -5647,8 +6692,14 @@
       <c r="H166">
         <v>14100</v>
       </c>
-    </row>
-    <row r="167" spans="1:8">
+      <c r="I166">
+        <v>1</v>
+      </c>
+      <c r="J166">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10">
       <c r="A167">
         <v>165</v>
       </c>
@@ -5673,8 +6724,14 @@
       <c r="H167">
         <v>14100</v>
       </c>
-    </row>
-    <row r="168" spans="1:8">
+      <c r="I167">
+        <v>1</v>
+      </c>
+      <c r="J167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10">
       <c r="A168">
         <v>166</v>
       </c>
@@ -5699,8 +6756,14 @@
       <c r="H168">
         <v>14100</v>
       </c>
-    </row>
-    <row r="169" spans="1:8">
+      <c r="I168">
+        <v>1</v>
+      </c>
+      <c r="J168">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10">
       <c r="A169">
         <v>167</v>
       </c>
@@ -5725,8 +6788,14 @@
       <c r="H169">
         <v>14100</v>
       </c>
-    </row>
-    <row r="170" spans="1:8">
+      <c r="I169">
+        <v>1</v>
+      </c>
+      <c r="J169">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10">
       <c r="A170">
         <v>168</v>
       </c>
@@ -5751,8 +6820,14 @@
       <c r="H170">
         <v>14100</v>
       </c>
-    </row>
-    <row r="171" spans="1:8">
+      <c r="I170">
+        <v>1</v>
+      </c>
+      <c r="J170">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10">
       <c r="A171">
         <v>169</v>
       </c>
@@ -5777,8 +6852,14 @@
       <c r="H171">
         <v>14100</v>
       </c>
-    </row>
-    <row r="172" spans="1:8">
+      <c r="I171">
+        <v>1</v>
+      </c>
+      <c r="J171">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10">
       <c r="A172">
         <v>170</v>
       </c>
@@ -5803,8 +6884,14 @@
       <c r="H172">
         <v>14100</v>
       </c>
-    </row>
-    <row r="173" spans="1:8">
+      <c r="I172">
+        <v>1</v>
+      </c>
+      <c r="J172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10">
       <c r="A173">
         <v>171</v>
       </c>
@@ -5829,8 +6916,14 @@
       <c r="H173">
         <v>14100</v>
       </c>
-    </row>
-    <row r="174" spans="1:8">
+      <c r="I173">
+        <v>1</v>
+      </c>
+      <c r="J173">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:10">
       <c r="A174">
         <v>172</v>
       </c>
@@ -5855,8 +6948,14 @@
       <c r="H174">
         <v>14100</v>
       </c>
-    </row>
-    <row r="175" spans="1:8">
+      <c r="I174">
+        <v>1</v>
+      </c>
+      <c r="J174">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10">
       <c r="A175">
         <v>173</v>
       </c>
@@ -5881,8 +6980,14 @@
       <c r="H175">
         <v>14100</v>
       </c>
-    </row>
-    <row r="176" spans="1:8">
+      <c r="I175">
+        <v>1</v>
+      </c>
+      <c r="J175">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:10">
       <c r="A176">
         <v>174</v>
       </c>
@@ -5907,8 +7012,14 @@
       <c r="H176">
         <v>14100</v>
       </c>
-    </row>
-    <row r="177" spans="1:8">
+      <c r="I176">
+        <v>1</v>
+      </c>
+      <c r="J176">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10">
       <c r="A177">
         <v>175</v>
       </c>
@@ -5933,8 +7044,14 @@
       <c r="H177">
         <v>14100</v>
       </c>
-    </row>
-    <row r="178" spans="1:8">
+      <c r="I177">
+        <v>1</v>
+      </c>
+      <c r="J177">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:10">
       <c r="A178">
         <v>176</v>
       </c>
@@ -5959,8 +7076,14 @@
       <c r="H178">
         <v>14100</v>
       </c>
-    </row>
-    <row r="179" spans="1:8">
+      <c r="I178">
+        <v>1</v>
+      </c>
+      <c r="J178">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:10">
       <c r="A179">
         <v>177</v>
       </c>
@@ -5985,8 +7108,14 @@
       <c r="H179">
         <v>14100</v>
       </c>
-    </row>
-    <row r="180" spans="1:8">
+      <c r="I179">
+        <v>1</v>
+      </c>
+      <c r="J179">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:10">
       <c r="A180">
         <v>178</v>
       </c>
@@ -6011,8 +7140,14 @@
       <c r="H180">
         <v>14100</v>
       </c>
-    </row>
-    <row r="181" spans="1:8">
+      <c r="I180">
+        <v>1</v>
+      </c>
+      <c r="J180">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:10">
       <c r="A181">
         <v>179</v>
       </c>
@@ -6037,8 +7172,14 @@
       <c r="H181">
         <v>14100</v>
       </c>
-    </row>
-    <row r="182" spans="1:8">
+      <c r="I181">
+        <v>1</v>
+      </c>
+      <c r="J181">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10">
       <c r="A182">
         <v>180</v>
       </c>
@@ -6063,8 +7204,14 @@
       <c r="H182">
         <v>14100</v>
       </c>
-    </row>
-    <row r="183" spans="1:8">
+      <c r="I182">
+        <v>1</v>
+      </c>
+      <c r="J182">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:10">
       <c r="A183">
         <v>181</v>
       </c>
@@ -6089,8 +7236,14 @@
       <c r="H183">
         <v>14100</v>
       </c>
-    </row>
-    <row r="184" spans="1:8">
+      <c r="I183">
+        <v>1</v>
+      </c>
+      <c r="J183">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:10">
       <c r="A184">
         <v>182</v>
       </c>
@@ -6115,8 +7268,14 @@
       <c r="H184">
         <v>14100</v>
       </c>
-    </row>
-    <row r="185" spans="1:8">
+      <c r="I184">
+        <v>1</v>
+      </c>
+      <c r="J184">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:10">
       <c r="A185">
         <v>183</v>
       </c>
@@ -6141,8 +7300,14 @@
       <c r="H185">
         <v>14100</v>
       </c>
-    </row>
-    <row r="186" spans="1:8">
+      <c r="I185">
+        <v>1</v>
+      </c>
+      <c r="J185">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10">
       <c r="A186">
         <v>184</v>
       </c>
@@ -6167,8 +7332,14 @@
       <c r="H186">
         <v>14100</v>
       </c>
-    </row>
-    <row r="187" spans="1:8">
+      <c r="I186">
+        <v>1</v>
+      </c>
+      <c r="J186">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:10">
       <c r="A187">
         <v>185</v>
       </c>
@@ -6193,8 +7364,14 @@
       <c r="H187">
         <v>14100</v>
       </c>
-    </row>
-    <row r="188" spans="1:8">
+      <c r="I187">
+        <v>1</v>
+      </c>
+      <c r="J187">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10">
       <c r="A188">
         <v>186</v>
       </c>
@@ -6219,8 +7396,14 @@
       <c r="H188">
         <v>14100</v>
       </c>
-    </row>
-    <row r="189" spans="1:8">
+      <c r="I188">
+        <v>1</v>
+      </c>
+      <c r="J188">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10">
       <c r="A189">
         <v>187</v>
       </c>
@@ -6245,8 +7428,14 @@
       <c r="H189">
         <v>14100</v>
       </c>
-    </row>
-    <row r="190" spans="1:8">
+      <c r="I189">
+        <v>1</v>
+      </c>
+      <c r="J189">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:10">
       <c r="A190">
         <v>188</v>
       </c>
@@ -6271,8 +7460,14 @@
       <c r="H190">
         <v>14100</v>
       </c>
-    </row>
-    <row r="191" spans="1:8">
+      <c r="I190">
+        <v>1</v>
+      </c>
+      <c r="J190">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10">
       <c r="A191">
         <v>189</v>
       </c>
@@ -6297,8 +7492,14 @@
       <c r="H191">
         <v>14100</v>
       </c>
-    </row>
-    <row r="192" spans="1:8">
+      <c r="I191">
+        <v>1</v>
+      </c>
+      <c r="J191">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10">
       <c r="A192">
         <v>190</v>
       </c>
@@ -6323,8 +7524,14 @@
       <c r="H192">
         <v>14100</v>
       </c>
-    </row>
-    <row r="193" spans="1:8">
+      <c r="I192">
+        <v>1</v>
+      </c>
+      <c r="J192">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:10">
       <c r="A193">
         <v>191</v>
       </c>
@@ -6349,8 +7556,14 @@
       <c r="H193">
         <v>14100</v>
       </c>
-    </row>
-    <row r="194" spans="1:8">
+      <c r="I193">
+        <v>1</v>
+      </c>
+      <c r="J193">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:10">
       <c r="A194">
         <v>192</v>
       </c>
@@ -6375,8 +7588,14 @@
       <c r="H194">
         <v>14100</v>
       </c>
-    </row>
-    <row r="195" spans="1:8">
+      <c r="I194">
+        <v>1</v>
+      </c>
+      <c r="J194">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:10">
       <c r="A195">
         <v>193</v>
       </c>
@@ -6401,8 +7620,14 @@
       <c r="H195">
         <v>14100</v>
       </c>
-    </row>
-    <row r="196" spans="1:8">
+      <c r="I195">
+        <v>1</v>
+      </c>
+      <c r="J195">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:10">
       <c r="A196">
         <v>194</v>
       </c>
@@ -6427,8 +7652,14 @@
       <c r="H196">
         <v>14100</v>
       </c>
-    </row>
-    <row r="197" spans="1:8">
+      <c r="I196">
+        <v>1</v>
+      </c>
+      <c r="J196">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:10">
       <c r="A197">
         <v>195</v>
       </c>
@@ -6453,8 +7684,14 @@
       <c r="H197">
         <v>14100</v>
       </c>
-    </row>
-    <row r="198" spans="1:8">
+      <c r="I197">
+        <v>1</v>
+      </c>
+      <c r="J197">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:10">
       <c r="A198">
         <v>196</v>
       </c>
@@ -6479,8 +7716,14 @@
       <c r="H198">
         <v>14100</v>
       </c>
-    </row>
-    <row r="199" spans="1:8">
+      <c r="I198">
+        <v>1</v>
+      </c>
+      <c r="J198">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:10">
       <c r="A199">
         <v>197</v>
       </c>
@@ -6505,8 +7748,14 @@
       <c r="H199">
         <v>14100</v>
       </c>
-    </row>
-    <row r="200" spans="1:8">
+      <c r="I199">
+        <v>1</v>
+      </c>
+      <c r="J199">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:10">
       <c r="A200">
         <v>198</v>
       </c>
@@ -6531,8 +7780,14 @@
       <c r="H200">
         <v>14100</v>
       </c>
-    </row>
-    <row r="201" spans="1:8">
+      <c r="I200">
+        <v>1</v>
+      </c>
+      <c r="J200">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:10">
       <c r="A201">
         <v>199</v>
       </c>
@@ -6557,8 +7812,14 @@
       <c r="H201">
         <v>14100</v>
       </c>
-    </row>
-    <row r="202" spans="1:8">
+      <c r="I201">
+        <v>1</v>
+      </c>
+      <c r="J201">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:10">
       <c r="A202">
         <v>200</v>
       </c>
@@ -6583,8 +7844,14 @@
       <c r="H202">
         <v>14100</v>
       </c>
-    </row>
-    <row r="203" spans="1:8">
+      <c r="I202">
+        <v>1</v>
+      </c>
+      <c r="J202">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:10">
       <c r="A203">
         <v>201</v>
       </c>
@@ -6609,8 +7876,14 @@
       <c r="H203">
         <v>14100</v>
       </c>
-    </row>
-    <row r="204" spans="1:8">
+      <c r="I203">
+        <v>1</v>
+      </c>
+      <c r="J203">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:10">
       <c r="A204">
         <v>202</v>
       </c>
@@ -6621,7 +7894,7 @@
         <v>201</v>
       </c>
       <c r="D204">
-        <f t="shared" ref="D196:D210" si="2">E204</f>
+        <f t="shared" ref="D204:D210" si="2">E204</f>
         <v>3</v>
       </c>
       <c r="E204">
@@ -6636,8 +7909,14 @@
       <c r="H204">
         <v>14100</v>
       </c>
-    </row>
-    <row r="205" spans="1:8">
+      <c r="I204">
+        <v>1</v>
+      </c>
+      <c r="J204">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:10">
       <c r="A205">
         <v>203</v>
       </c>
@@ -6663,8 +7942,14 @@
       <c r="H205">
         <v>14100</v>
       </c>
-    </row>
-    <row r="206" spans="1:8">
+      <c r="I205">
+        <v>1</v>
+      </c>
+      <c r="J205">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:10">
       <c r="A206">
         <v>204</v>
       </c>
@@ -6690,8 +7975,14 @@
       <c r="H206">
         <v>14100</v>
       </c>
-    </row>
-    <row r="207" spans="1:8">
+      <c r="I206">
+        <v>1</v>
+      </c>
+      <c r="J206">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:10">
       <c r="A207">
         <v>205</v>
       </c>
@@ -6717,8 +8008,14 @@
       <c r="H207">
         <v>14100</v>
       </c>
-    </row>
-    <row r="208" spans="1:8">
+      <c r="I207">
+        <v>1</v>
+      </c>
+      <c r="J207">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:10">
       <c r="A208">
         <v>206</v>
       </c>
@@ -6744,8 +8041,14 @@
       <c r="H208">
         <v>14100</v>
       </c>
-    </row>
-    <row r="209" spans="1:8">
+      <c r="I208">
+        <v>1</v>
+      </c>
+      <c r="J208">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:10">
       <c r="A209">
         <v>207</v>
       </c>
@@ -6771,8 +8074,14 @@
       <c r="H209">
         <v>14100</v>
       </c>
-    </row>
-    <row r="210" spans="1:8">
+      <c r="I209">
+        <v>1</v>
+      </c>
+      <c r="J209">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:10">
       <c r="A210">
         <v>208</v>
       </c>
@@ -6797,6 +8106,12 @@
       </c>
       <c r="H210">
         <v>14100</v>
+      </c>
+      <c r="I210">
+        <v>1</v>
+      </c>
+      <c r="J210">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Equip ship header part2, including demon shipheader
</commit_message>
<xml_diff>
--- a/DataSource/excel/Item.xlsx
+++ b/DataSource/excel/Item.xlsx
@@ -30,6 +30,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Yujie Liu</author>
+    <author>YujieLiu</author>
   </authors>
   <commentList>
     <comment ref="D1" authorId="0">
@@ -151,6 +152,28 @@
         </r>
       </text>
     </comment>
+    <comment ref="F124" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>YujieLiu:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+无法拆除</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -828,7 +851,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -878,6 +901,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1273,8 +1307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J210"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G117" sqref="G117"/>
+    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
+      <selection activeCell="J124" sqref="J124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5350,7 +5384,7 @@
         <v>6</v>
       </c>
       <c r="F124">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G124">
         <v>0</v>

</xml_diff>

<commit_message>
Add big bird shipheader function
</commit_message>
<xml_diff>
--- a/DataSource/excel/Item.xlsx
+++ b/DataSource/excel/Item.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27309"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27610"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15860" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Item.csv" sheetId="1" r:id="rId1"/>
@@ -1307,8 +1307,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
-      <selection activeCell="J124" sqref="J124"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B97" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="B126" sqref="B126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5160,7 +5163,7 @@
         <v>6</v>
       </c>
       <c r="F117">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G117">
         <v>0</v>
@@ -5192,7 +5195,7 @@
         <v>6</v>
       </c>
       <c r="F118">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G118">
         <v>0</v>
@@ -5224,7 +5227,7 @@
         <v>6</v>
       </c>
       <c r="F119">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G119">
         <v>0</v>
@@ -5256,7 +5259,7 @@
         <v>6</v>
       </c>
       <c r="F120">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G120">
         <v>0</v>
@@ -5288,7 +5291,7 @@
         <v>6</v>
       </c>
       <c r="F121">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G121">
         <v>0</v>
@@ -5320,7 +5323,7 @@
         <v>6</v>
       </c>
       <c r="F122">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G122">
         <v>0</v>
@@ -5352,7 +5355,7 @@
         <v>6</v>
       </c>
       <c r="F123">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G123">
         <v>0</v>
@@ -5416,7 +5419,7 @@
         <v>6</v>
       </c>
       <c r="F125">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G125">
         <v>0</v>
@@ -5448,7 +5451,7 @@
         <v>6</v>
       </c>
       <c r="F126">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G126">
         <v>0</v>

</xml_diff>